<commit_message>
update readme.pdf and samples
</commit_message>
<xml_diff>
--- a/samples/csv_file__address__four_fields/Locations.xlsx
+++ b/samples/csv_file__address__four_fields/Locations.xlsx
@@ -14,19 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Icon_color</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>Thumb_URL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
   <si>
     <t>R</t>
   </si>
@@ -127,24 +115,12 @@
     <t>http://farm8.staticflickr.com/7074/6855416852_da59fd8a73_m.jpg</t>
   </si>
   <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
     <t>New York's cool new park in the sky</t>
   </si>
   <si>
     <t>http://farm8.staticflickr.com/7062/6855356176_f7f5801fd5_b.jpg</t>
   </si>
   <si>
-    <t>Hovering above Manhattan's West Side on a formerly abandoned elevated railroad is an aerial park that has become one of New York City's top attractions.</t>
-  </si>
-  <si>
     <t>New York</t>
   </si>
   <si>
@@ -160,9 +136,6 @@
     <t>95 Gansevoort Street</t>
   </si>
   <si>
-    <t>Zipcode</t>
-  </si>
-  <si>
     <t>509 W 29th Street</t>
   </si>
   <si>
@@ -181,7 +154,37 @@
     <t>478 W 15th Street</t>
   </si>
   <si>
-    <t>Caption</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>caption</t>
+  </si>
+  <si>
+    <t>icon_color</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>pic_url</t>
+  </si>
+  <si>
+    <t>thumb_url</t>
+  </si>
+  <si>
+    <t>http://farm8.staticflickr.com/7062/6855356176_f7f5801fd5_m.jpg</t>
+  </si>
+  <si>
+    <t>Hovering above Manhattan's West Side on a formerly abandoned elevated railroad is an aerial park that has become one of New York City's top attractions. &lt;i&gt;&lt;a href="http://www.thehighline.org" style="color:yellow" target="_blank"&gt;More Info&lt;/a&gt;&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>zip</t>
   </si>
 </sst>
 </file>
@@ -666,13 +669,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1019,7 +1025,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1035,286 +1041,292 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G2" s="1">
         <v>10001</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>41</v>
+      <c r="H2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G3" s="1">
         <v>10011</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>7</v>
+      <c r="H3" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G4" s="1">
         <v>10011</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G5" s="1">
         <v>10011</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G6" s="1">
         <v>10011</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G7" s="1">
         <v>10011</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G8" s="1">
         <v>10014</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G9" s="1">
         <v>10014</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G10" s="1">
         <v>10014</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>